<commit_message>
Including name operator on well excel import
</commit_message>
<xml_diff>
--- a/test/data/wells.xlsx
+++ b/test/data/wells.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="44">
   <si>
     <t>poco</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>Albacora</t>
+  </si>
+  <si>
+    <t>Nome operador</t>
+  </si>
+  <si>
+    <t>poço</t>
   </si>
 </sst>
 </file>
@@ -514,239 +520,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="9" max="9" width="25.125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.125" customWidth="1"/>
+    <col min="15" max="15" width="10.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>-12.794294000000001</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>-38.436382000000002</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>42248</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>-9.9879960000000008</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>-38.676555999999998</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>42734</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>-4.9180859999999997</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>-37.224645000000002</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <v>40931</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>29</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>30</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>29</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>30</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>29</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>30</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>35</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>36</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>37</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>38</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>36</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>38</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>36</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>41</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>36</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>